<commit_message>
Feat(/exercices/linked-list/): finished in 10 min
</commit_message>
<xml_diff>
--- a/Suivi_Projet.xlsx
+++ b/Suivi_Projet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>TerminÃ©</t>
+  </si>
+  <si>
+    <t>19.12.2025 16:03</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -118,6 +121,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Feat(./exercices/rna-transcription/): finished in 20 min
</commit_message>
<xml_diff>
--- a/Suivi_Projet.xlsx
+++ b/Suivi_Projet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>19.12.2025 16:03</t>
+  </si>
+  <si>
+    <t>09.01.2026 12:45</t>
+  </si>
+  <si>
+    <t>Termine</t>
   </si>
 </sst>
 </file>
@@ -81,7 +87,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -135,6 +141,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>